<commit_message>
Store Plan for zero-doc
</commit_message>
<xml_diff>
--- a/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.directory.xlsx
+++ b/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/web-app/workshop/zero-ws/zero-extension/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB31F956-84A1-324C-81CA-4616A48DF407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AF69E2-C24A-1140-8EAE-B67BB67F0393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45720" yWindow="-6760" windowWidth="38400" windowHeight="16940" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="1700" yWindow="5040" windowWidth="34160" windowHeight="41960" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-CDATA" sheetId="7" r:id="rId1"/>
@@ -157,19 +157,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>JSON:cab/directory/service.catalog.json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JSON:cab/directory/system.document.json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>系统文档</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>io.horizon.spi.feature.CatalogArbor</t>
+  </si>
+  <si>
+    <t>JSON:cab/directory/ambient.dir.document.json</t>
+  </si>
+  <si>
+    <t>JSON:cab/directory/ambient.dir.workflow.json</t>
   </si>
 </sst>
 </file>
@@ -710,7 +708,7 @@
   <dimension ref="A2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -725,7 +723,7 @@
     <col min="8" max="8" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="52.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="56.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -826,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>28</v>
@@ -844,10 +842,10 @@
         <v>21</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="66" x14ac:dyDescent="0.2">
@@ -877,10 +875,10 @@
         <v>21</v>
       </c>
       <c r="J6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>